<commit_message>
antes de empezar el scrapping masivo
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Desktop\web-scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F41F2-2CAE-4F67-8866-C8465F3F186D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88389544-1844-4229-B4FE-2546D43DDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -43,13 +43,16 @@
     <t>image_url</t>
   </si>
   <si>
-    <t>4504399400</t>
-  </si>
-  <si>
-    <t>Pack De 6 Unidades De Soda Cocacola 600 ML</t>
-  </si>
-  <si>
-    <t>$ 4.74</t>
+    <t>pos_categ_id</t>
+  </si>
+  <si>
+    <t>7452000201667</t>
+  </si>
+  <si>
+    <t>Nuggets Regular Muslo Toledano 340 gr</t>
+  </si>
+  <si>
+    <t>2.79</t>
   </si>
   <si>
     <t>EXENTO</t>
@@ -58,19 +61,22 @@
     <t>0.00</t>
   </si>
   <si>
-    <t>https://superxtrapanama.vtexassets.com/arquivos/ids/189436-800-auto?v=638507112319470000&amp;width=800&amp;height=auto&amp;aspect=true</t>
-  </si>
-  <si>
-    <t>7445072006551</t>
-  </si>
-  <si>
-    <t>Jugo Cifrut Naranja Mandarina Limon 3030 Ml</t>
-  </si>
-  <si>
-    <t>$ 1.76</t>
-  </si>
-  <si>
-    <t>https://superxtrapanama.vtexassets.com/arquivos/ids/191377-800-auto?v=638550589268830000&amp;width=800&amp;height=auto&amp;aspect=true</t>
+    <t>https://superxtrapanama.vtexassets.com/arquivos/ids/158309-800-auto?v=637806395111300000&amp;width=800&amp;height=auto&amp;aspect=true</t>
+  </si>
+  <si>
+    <t>Congelados</t>
+  </si>
+  <si>
+    <t>8711786256483</t>
+  </si>
+  <si>
+    <t>Papas Cong Chefs Best 2 5 Kg</t>
+  </si>
+  <si>
+    <t>5.49</t>
+  </si>
+  <si>
+    <t>https://superxtrapanama.vtexassets.com/arquivos/ids/191442-800-auto?v=638551093696600000&amp;width=800&amp;height=auto&amp;aspect=true</t>
   </si>
 </sst>
 </file>
@@ -433,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,45 +469,54 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>